<commit_message>
First Three exercise done.
</commit_message>
<xml_diff>
--- a/CSVStats.xlsx
+++ b/CSVStats.xlsx
@@ -508,7 +508,7 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -564,46 +564,100 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9">
+        <v>205</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>10</v>
       </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>11</v>
       </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>12</v>
       </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
@@ -630,61 +684,121 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>2</v>
       </c>
+      <c r="C17">
+        <v>155</v>
+      </c>
+      <c r="D17">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>4</v>
       </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>5</v>
       </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>6</v>
       </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>7</v>
       </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
         <v>8</v>
       </c>
+      <c r="C22">
+        <v>105</v>
+      </c>
+      <c r="D22">
+        <v>70</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
         <v>9</v>
       </c>
+      <c r="C23">
+        <v>240</v>
+      </c>
+      <c r="D23">
+        <v>160</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
         <v>10</v>
       </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>11</v>
       </c>
+      <c r="C25">
+        <v>150</v>
+      </c>
+      <c r="D25">
+        <v>150</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>12</v>
       </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
@@ -711,61 +825,121 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>175</v>
+        <v>250</v>
       </c>
       <c r="D30">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
         <v>2</v>
       </c>
+      <c r="C31">
+        <v>185</v>
+      </c>
+      <c r="D31">
+        <v>115</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
         <v>4</v>
       </c>
+      <c r="C32">
+        <v>130</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>5</v>
       </c>
+      <c r="C33">
+        <v>25</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>6</v>
       </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="B35" t="s">
         <v>7</v>
       </c>
+      <c r="C35">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="B36" t="s">
         <v>8</v>
       </c>
+      <c r="C36">
+        <v>130</v>
+      </c>
+      <c r="D36">
+        <v>75</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" t="s">
         <v>9</v>
       </c>
+      <c r="C37">
+        <v>295</v>
+      </c>
+      <c r="D37">
+        <v>190</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="B38" t="s">
         <v>10</v>
       </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="B39" t="s">
         <v>11</v>
       </c>
+      <c r="C39">
+        <v>190</v>
+      </c>
+      <c r="D39">
+        <v>190</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="B40" t="s">
         <v>12</v>
       </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>25</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
@@ -790,12 +964,6 @@
       </c>
       <c r="B44" t="s">
         <v>3</v>
-      </c>
-      <c r="C44">
-        <v>175</v>
-      </c>
-      <c r="D44">
-        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:5">

</xml_diff>